<commit_message>
Update project files including hardware, models, scripts and documentation
</commit_message>
<xml_diff>
--- a/output/se_comparison/se_comparison_results.xlsx
+++ b/output/se_comparison/se_comparison_results.xlsx
@@ -498,87 +498,87 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MicroPizzaNet (Original)</t>
+          <t>MicroPizzaNetWithSE (SE-Ratio=8)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41.66666666666667</v>
+        <v>25</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4242424242424243</v>
+        <v>0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5625</v>
+        <v>0.0625</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="F2" t="n">
-        <v>582</v>
+        <v>662</v>
       </c>
       <c r="G2" t="n">
-        <v>2.53515625</v>
+        <v>2.84765625</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6337890625</v>
+        <v>0.7119140625</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1268219947814941</v>
+        <v>0.2221250534057617</v>
       </c>
       <c r="J2" t="n">
-        <v>4.438769817352295</v>
+        <v>7.77437686920166</v>
       </c>
       <c r="K2" t="n">
-        <v>102.0947265625</v>
+        <v>102.3837890625</v>
       </c>
       <c r="L2" t="n">
-        <v>3.23222279548645</v>
+        <v>6.081669807434082</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MicroPizzaNetWithSE (SE-Ratio=4)</t>
+          <t>MicroPizzaNet (Original)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>8.333333333333332</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F3" t="n">
-        <v>742</v>
+        <v>582</v>
       </c>
       <c r="G3" t="n">
-        <v>3.16015625</v>
+        <v>2.53515625</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7900390625</v>
+        <v>0.6337890625</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2217984199523926</v>
+        <v>0.1268362998962402</v>
       </c>
       <c r="J3" t="n">
-        <v>7.762944698333739</v>
+        <v>4.439270496368408</v>
       </c>
       <c r="K3" t="n">
-        <v>102.4853515625</v>
+        <v>102.0947265625</v>
       </c>
       <c r="L3" t="n">
-        <v>3.122381210327148</v>
+        <v>5.852807760238647</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MicroPizzaNetWithSE (SE-Ratio=8)</t>
+          <t>MicroPizzaNetWithSE (SE-Ratio=4)</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -594,25 +594,25 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>662</v>
+        <v>742</v>
       </c>
       <c r="G4" t="n">
-        <v>2.84765625</v>
+        <v>3.16015625</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7119140625</v>
+        <v>0.7900390625</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2202010154724121</v>
+        <v>0.2347159385681152</v>
       </c>
       <c r="J4" t="n">
-        <v>7.707035541534424</v>
+        <v>8.215057849884035</v>
       </c>
       <c r="K4" t="n">
-        <v>102.3837890625</v>
+        <v>102.4853515625</v>
       </c>
       <c r="L4" t="n">
-        <v>3.19222617149353</v>
+        <v>5.895447731018066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>